<commit_message>
start time and end time logic is missing
</commit_message>
<xml_diff>
--- a/solar-plant.xlsx
+++ b/solar-plant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4th_Dimension\Desktop\ArjunTask\WeatherMeterManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7BD454-6D13-4968-A807-08842B061176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4478865-FFB9-474E-87F7-3C6B21B65A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6450" yWindow="3825" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>dgdggg</t>
+  </si>
+  <si>
+    <t>hgujfghuyfv</t>
+  </si>
+  <si>
+    <t>hghghg</t>
   </si>
 </sst>
 </file>
@@ -626,7 +632,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1563,8 +1569,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="36" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="37" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:1" ht="14.25" customHeight="1"/>

</xml_diff>